<commit_message>
Updated PC communications protocol
</commit_message>
<xml_diff>
--- a/Current Cycling/Current Cycling Cabinet PCB Design.xlsx
+++ b/Current Cycling/Current Cycling Cabinet PCB Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Projects\Current Cycling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3737C51D-6802-4AEA-A3E4-D44183CA9B69}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE21CA-49D4-48E0-AABA-451289ECFE78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7669683-8C58-47AD-AB59-72FC40B2BAC7}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="399">
   <si>
     <t>Assembly</t>
   </si>
@@ -1222,9 +1222,6 @@
     <t>Temp 16</t>
   </si>
   <si>
-    <t>Binary</t>
-  </si>
-  <si>
     <t>3 bit - indicates which smoke sensor is used</t>
   </si>
   <si>
@@ -1235,6 +1232,12 @@
   </si>
   <si>
     <t>Active Temp Sensor</t>
+  </si>
+  <si>
+    <t>Beginning of string needs to have a "&lt;" and end of string needs to have a "&gt;"</t>
+  </si>
+  <si>
+    <t>Example: &lt;75.0,3.5,70,50,1,0,0,13,4&gt;</t>
   </si>
 </sst>
 </file>
@@ -1715,10 +1718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0917387-7D6B-4A20-A541-790136947EE9}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1738,42 +1741,30 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
     </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>346</v>
-      </c>
-      <c r="B4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C4" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="C5" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>385</v>
+        <v>346</v>
       </c>
       <c r="B6" t="s">
         <v>352</v>
@@ -1784,126 +1775,114 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="B7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>352</v>
       </c>
       <c r="C7" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>384</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
+      </c>
+      <c r="B8" t="s">
+        <v>352</v>
       </c>
       <c r="C8" t="s">
-        <v>391</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="B9" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B9" t="s">
+        <v>352</v>
+      </c>
+      <c r="C9" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>384</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="C9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>393</v>
-      </c>
       <c r="C10" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C11" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>396</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C12" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C13" t="s">
         <v>393</v>
       </c>
-      <c r="C11" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>354</v>
-      </c>
-      <c r="B16" t="s">
-        <v>352</v>
-      </c>
-      <c r="C16" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="B17" t="s">
-        <v>352</v>
-      </c>
-      <c r="C17" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B18" t="s">
-        <v>352</v>
-      </c>
-      <c r="C18" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="B19" t="s">
-        <v>352</v>
-      </c>
-      <c r="C19" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B20" t="s">
         <v>352</v>
@@ -1914,7 +1893,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B21" t="s">
         <v>352</v>
@@ -1925,7 +1904,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B22" t="s">
         <v>352</v>
@@ -1936,7 +1915,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B23" t="s">
         <v>352</v>
@@ -1947,7 +1926,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B24" t="s">
         <v>352</v>
@@ -1958,7 +1937,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B25" t="s">
         <v>352</v>
@@ -1969,7 +1948,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B26" t="s">
         <v>352</v>
@@ -1980,7 +1959,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B27" t="s">
         <v>352</v>
@@ -1991,7 +1970,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B28" t="s">
         <v>352</v>
@@ -2002,7 +1981,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B29" t="s">
         <v>352</v>
@@ -2013,7 +1992,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B30" t="s">
         <v>352</v>
@@ -2023,8 +2002,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>392</v>
+      <c r="A31" s="5" t="s">
+        <v>365</v>
       </c>
       <c r="B31" t="s">
         <v>352</v>
@@ -2035,51 +2014,51 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B32" t="s">
         <v>352</v>
       </c>
       <c r="C32" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>371</v>
+      <c r="A33" s="5" t="s">
+        <v>367</v>
       </c>
       <c r="B33" t="s">
         <v>352</v>
       </c>
       <c r="C33" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B34" t="s">
         <v>352</v>
       </c>
       <c r="C34" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>373</v>
+        <v>392</v>
       </c>
       <c r="B35" t="s">
         <v>352</v>
       </c>
       <c r="C35" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B36" t="s">
         <v>352</v>
@@ -2090,7 +2069,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B37" t="s">
         <v>352</v>
@@ -2101,7 +2080,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B38" t="s">
         <v>352</v>
@@ -2112,7 +2091,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B39" t="s">
         <v>352</v>
@@ -2123,33 +2102,77 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B40" t="s">
-        <v>379</v>
+        <v>352</v>
+      </c>
+      <c r="C40" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="B41" t="s">
-        <v>379</v>
+        <v>352</v>
+      </c>
+      <c r="C41" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B42" t="s">
-        <v>379</v>
+        <v>352</v>
+      </c>
+      <c r="C42" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>377</v>
+      </c>
+      <c r="B43" t="s">
+        <v>352</v>
+      </c>
+      <c r="C43" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>378</v>
+      </c>
+      <c r="B44" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>380</v>
+      </c>
+      <c r="B45" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>383</v>
+      </c>
+      <c r="B46" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>390</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B47" t="s">
         <v>379</v>
       </c>
     </row>

</xml_diff>